<commit_message>
updating metadata with bowtie2 percent match to reference genome
</commit_message>
<xml_diff>
--- a/data/metadata_host_flower_genomes.xlsx
+++ b/data/metadata_host_flower_genomes.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garci\AppData\Local\Temp\fz3temp-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7476250C-375C-4CFC-9A10-1EADEBFC6C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0B4383-588A-4BBD-94F5-467D7C80000B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7810" yWindow="0" windowWidth="11480" windowHeight="11370" activeTab="2" xr2:uid="{9C6DCD7B-FBCB-4AA0-BC7B-8223D9C72C5E}"/>
+    <workbookView xWindow="7810" yWindow="0" windowWidth="11480" windowHeight="11370" firstSheet="3" activeTab="3" xr2:uid="{9C6DCD7B-FBCB-4AA0-BC7B-8223D9C72C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="sequenced" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Ref genome links" sheetId="4" r:id="rId3"/>
+    <sheet name="Bowtie2 alignment percent" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$A$1:$E$101</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="216">
   <si>
     <t>Sample</t>
   </si>
@@ -684,6 +686,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>alignment percent</t>
   </si>
 </sst>
 </file>
@@ -740,7 +745,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +761,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEED6E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -800,6 +859,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -807,6 +887,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEED6E8"/>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2807,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF299B7B-B1AA-F747-B371-AE9D9BECA23B}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="D36" zoomScale="121" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView topLeftCell="D1" zoomScale="44" workbookViewId="0">
+      <selection activeCell="M56" sqref="A1:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4288,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A323FCB9-156D-4942-B446-A6110CB73782}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="B1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4732,4 +4820,1484 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E13B2E-36F9-44E2-B939-6E89842AF962}">
+  <dimension ref="A1:J57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="88" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.54296875" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7265625" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="11">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6">
+        <v>1.52</v>
+      </c>
+      <c r="J1" s="6">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>40</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>1.43</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>52</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
+        <v>1.18</v>
+      </c>
+      <c r="J4" s="6">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>63</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="J6" s="6">
+        <v>24.83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>64</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="J7" s="6">
+        <v>23.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>68</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="J8" s="6">
+        <v>92.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6">
+        <v>69</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <v>1.03</v>
+      </c>
+      <c r="J9" s="6">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6">
+        <v>70</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J10" s="6">
+        <v>20.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6">
+        <v>71</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="6">
+        <v>30.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="J12" s="6">
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <v>2.35</v>
+      </c>
+      <c r="J13" s="6">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6">
+        <v>74</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J14" s="6">
+        <v>22.42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6">
+        <v>77</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="J15" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6">
+        <v>78</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
+        <v>1.34</v>
+      </c>
+      <c r="J16" s="6">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6">
+        <v>79</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6">
+        <v>80</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6">
+        <v>81</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
+        <v>82</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6">
+        <v>84</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6">
+        <v>1.72</v>
+      </c>
+      <c r="J21" s="6">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
+        <v>87</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="J22" s="6">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6">
+        <v>88</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="J23" s="6">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="11">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6">
+        <v>89</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6">
+        <v>3.21</v>
+      </c>
+      <c r="J24" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6">
+        <v>90</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J25" s="6">
+        <v>7.21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="11">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6">
+        <v>91</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="J26" s="6">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
+        <v>92</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6">
+        <v>1.63</v>
+      </c>
+      <c r="J27" s="6">
+        <v>20.62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="13">
+        <v>2</v>
+      </c>
+      <c r="B28" s="14">
+        <v>43</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="J28" s="14">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="13">
+        <v>2</v>
+      </c>
+      <c r="B29" s="14">
+        <v>44</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14">
+        <v>0.42</v>
+      </c>
+      <c r="J29" s="14">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="13">
+        <v>2</v>
+      </c>
+      <c r="B30" s="14">
+        <v>49</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14">
+        <v>8.68</v>
+      </c>
+      <c r="J30" s="14">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="13">
+        <v>2</v>
+      </c>
+      <c r="B31" s="14">
+        <v>61</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14">
+        <v>2.33</v>
+      </c>
+      <c r="J31" s="14">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="13">
+        <v>2</v>
+      </c>
+      <c r="B32" s="14">
+        <v>62</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="J32" s="14">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="13">
+        <v>2</v>
+      </c>
+      <c r="B33" s="14">
+        <v>66</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="J33" s="14">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="13">
+        <v>2</v>
+      </c>
+      <c r="B34" s="14">
+        <v>75</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="J34" s="14">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="13">
+        <v>2</v>
+      </c>
+      <c r="B35" s="14">
+        <v>85</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="J35" s="14">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="15">
+        <v>3</v>
+      </c>
+      <c r="B36" s="16">
+        <v>50</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16">
+        <v>9.07</v>
+      </c>
+      <c r="J36" s="16">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="15">
+        <v>3</v>
+      </c>
+      <c r="B37" s="16">
+        <v>53</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16">
+        <v>21.7</v>
+      </c>
+      <c r="J37" s="16">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="15">
+        <v>3</v>
+      </c>
+      <c r="B38" s="16">
+        <v>58</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16">
+        <v>20</v>
+      </c>
+      <c r="J38" s="16">
+        <v>4.96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="15">
+        <v>3</v>
+      </c>
+      <c r="B39" s="16">
+        <v>59</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16">
+        <v>11.4</v>
+      </c>
+      <c r="J39" s="16">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="15">
+        <v>3</v>
+      </c>
+      <c r="B40" s="16">
+        <v>83</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J40" s="16">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="17">
+        <v>4</v>
+      </c>
+      <c r="B41" s="18">
+        <v>42</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18">
+        <v>1.41</v>
+      </c>
+      <c r="J41" s="18">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="17">
+        <v>4</v>
+      </c>
+      <c r="B42" s="18">
+        <v>56</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="19">
+        <v>5</v>
+      </c>
+      <c r="B43" s="20">
+        <v>45</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20">
+        <v>7.37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="19">
+        <v>5</v>
+      </c>
+      <c r="B44" s="20">
+        <v>47</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20">
+        <v>6.11</v>
+      </c>
+      <c r="J44" s="20">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="19">
+        <v>5</v>
+      </c>
+      <c r="B45" s="20">
+        <v>57</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20">
+        <v>10.3</v>
+      </c>
+      <c r="J45" s="20">
+        <v>7.66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="21">
+        <v>6</v>
+      </c>
+      <c r="B46" s="22">
+        <v>51</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22">
+        <v>1.38</v>
+      </c>
+      <c r="J46" s="22">
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="21">
+        <v>6</v>
+      </c>
+      <c r="B47" s="22">
+        <v>86</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22">
+        <v>0.62</v>
+      </c>
+      <c r="J47" s="22">
+        <v>19.72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="23">
+        <v>7</v>
+      </c>
+      <c r="B48" s="24">
+        <v>55</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24">
+        <v>9.64</v>
+      </c>
+      <c r="J48" s="24">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="23">
+        <v>7</v>
+      </c>
+      <c r="B49" s="24">
+        <v>65</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="J49" s="24">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="25">
+        <v>8</v>
+      </c>
+      <c r="B50" s="26">
+        <v>39</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" s="25">
+        <v>8</v>
+      </c>
+      <c r="B51" s="26">
+        <v>41</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="27">
+        <v>2.38</v>
+      </c>
+      <c r="J51" s="26">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="25">
+        <v>8</v>
+      </c>
+      <c r="B52" s="26">
+        <v>46</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="25">
+        <v>8</v>
+      </c>
+      <c r="B53" s="26">
+        <v>76</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26">
+        <v>1.78</v>
+      </c>
+      <c r="J53" s="26">
+        <v>87.48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" s="30">
+        <v>9</v>
+      </c>
+      <c r="B54" s="31">
+        <v>54</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31">
+        <v>13.4</v>
+      </c>
+      <c r="J54" s="31">
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" s="30">
+        <v>9</v>
+      </c>
+      <c r="B55" s="31">
+        <v>67</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31">
+        <v>3.77</v>
+      </c>
+      <c r="J55" s="31">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="28">
+        <v>10</v>
+      </c>
+      <c r="B56" s="29">
+        <v>93</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29">
+        <v>1.9</v>
+      </c>
+      <c r="J56" s="29">
+        <v>55.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:I56">
+    <sortCondition ref="A1:A56"/>
+    <sortCondition ref="B1:B56"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7711F-CFFB-4D3E-A781-F9237620FE41}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>